<commit_message>
Update HomeScreen, AddTransaction, transactionsAction, categoryAction, action. Add new packeage
- Update HomeScreen and AddTransaction ' s  UI
- Drop table TRANSACDATE
- Update DumbData
- Install and new package:
  - @react-navigation/material-top-tabs
  - react-native-actions-sheet
  - react-native-month-year-picker
  - react-native-pager-view
  - react-native-screens (update)
  - react-native-tab-view
- Delete Alert at categoriesAction
- Remove convertDate()
- Add ADD_TRANSACTION action
</commit_message>
<xml_diff>
--- a/DumbData.xlsx
+++ b/DumbData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\react-native\ExpensesTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{07207450-7A8A-4BB0-8FA6-2C8A7EFEB9C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEA8FB9-5912-47E1-88B1-4454A87F8304}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="195" windowWidth="19440" windowHeight="15000" xr2:uid="{CD52594F-1F1F-4A80-AC0F-6362B4AE18F6}"/>
+    <workbookView xWindow="29925" yWindow="5775" windowWidth="14505" windowHeight="9000" xr2:uid="{CD52594F-1F1F-4A80-AC0F-6362B4AE18F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
@@ -136,10 +136,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="172" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +169,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -182,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -214,42 +221,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -571,7 +600,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -582,320 +611,321 @@
     <col min="4" max="4" width="4" customWidth="1"/>
     <col min="5" max="5" width="11.75" customWidth="1"/>
     <col min="7" max="7" width="20.75" customWidth="1"/>
+    <col min="8" max="8" width="10.875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.125" customWidth="1"/>
     <col min="11" max="11" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="E1" s="6" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="E1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="J1" s="3" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="J1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="3"/>
+      <c r="K1" s="10"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>1</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="3">
         <v>-5182000</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="11">
+        <v>44337</v>
+      </c>
+      <c r="J3" s="5">
         <v>1</v>
       </c>
-      <c r="J3" s="8">
-        <v>1</v>
-      </c>
-      <c r="K3" s="8">
+      <c r="K3" s="5">
         <v>1621555200</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>3</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <v>-160000</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="11">
+        <v>44427</v>
+      </c>
+      <c r="J4" s="5">
         <v>2</v>
       </c>
-      <c r="J4" s="8">
+      <c r="K4" s="5">
+        <v>1629331200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3">
         <v>2</v>
       </c>
-      <c r="K4" s="8">
-        <v>1629331200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="F5" s="3">
+        <v>-50000</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="12">
+        <v>44484</v>
+      </c>
+      <c r="J5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="K5" s="5">
+        <v>1634256000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="5">
-        <v>2</v>
-      </c>
-      <c r="F5" s="5">
+      <c r="E6" s="3">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3">
+        <v>500000</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="11">
+        <v>44340</v>
+      </c>
+      <c r="J6" s="7">
+        <v>4</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1634342400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="3">
+        <v>10</v>
+      </c>
+      <c r="F7" s="6">
+        <v>300000</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="11">
+        <v>44485</v>
+      </c>
+      <c r="J7" s="7">
+        <v>5</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1635120000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="3">
+        <v>9</v>
+      </c>
+      <c r="F8" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="11">
+        <v>44494</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="3">
+        <v>8</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1200000</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="13">
+        <v>44484</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="3">
+        <v>4</v>
+      </c>
+      <c r="F10" s="3">
+        <v>-22000</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="11">
+        <v>44485</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="3">
+        <v>6</v>
+      </c>
+      <c r="F11" s="3">
         <v>-50000</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="8">
-        <v>2</v>
-      </c>
-      <c r="J5" s="8">
-        <v>3</v>
-      </c>
-      <c r="K5" s="8">
-        <v>1634256000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="5">
-        <v>9</v>
-      </c>
-      <c r="F6" s="5">
-        <v>500000</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="8">
-        <v>3</v>
-      </c>
-      <c r="J6" s="10">
-        <v>4</v>
-      </c>
-      <c r="K6" s="5">
-        <v>1634342400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="5">
+      <c r="G11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="11">
+        <v>44345</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="F7" s="9">
-        <v>300000</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="5">
-        <v>4</v>
-      </c>
-      <c r="J7" s="10">
-        <v>5</v>
-      </c>
-      <c r="K7" s="1">
-        <v>1635120000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="5">
-        <v>9</v>
-      </c>
-      <c r="F8" s="5">
-        <v>10000</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="5">
-        <v>8</v>
-      </c>
-      <c r="F9" s="5">
-        <v>1200000</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="5">
-        <v>4</v>
-      </c>
-      <c r="F10" s="5">
-        <v>-22000</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
-        <v>9</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="5">
-        <v>6</v>
-      </c>
-      <c r="F11" s="5">
-        <v>-50000</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
+      <c r="D12" s="1"/>
+      <c r="E12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="5">
-        <v>10</v>
-      </c>
-      <c r="F12" s="5">
+      <c r="F12" s="3">
         <v>200000</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="5">
-        <v>5</v>
+      <c r="H12" s="11">
+        <v>44494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove TRANSACDATE's table, sort data in TRANSACTION by date
</commit_message>
<xml_diff>
--- a/DumbData.xlsx
+++ b/DumbData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\react-native\ExpensesTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEA8FB9-5912-47E1-88B1-4454A87F8304}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B659049-B256-43A7-93C7-266AA1739D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29925" yWindow="5775" windowWidth="14505" windowHeight="9000" xr2:uid="{CD52594F-1F1F-4A80-AC0F-6362B4AE18F6}"/>
+    <workbookView xWindow="2190" yWindow="3150" windowWidth="14400" windowHeight="10755" xr2:uid="{CD52594F-1F1F-4A80-AC0F-6362B4AE18F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>catetgory_id</t>
   </si>
@@ -45,9 +45,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>Học phí</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
   </si>
   <si>
     <t>income</t>
-  </si>
-  <si>
-    <t>TRANSACDATE</t>
   </si>
   <si>
     <t>Lãi</t>
@@ -138,7 +132,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="172" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -240,7 +234,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -254,13 +248,16 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
@@ -268,18 +265,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -597,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D37B0280-B365-4098-940E-D3F832A9360A}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -616,32 +601,28 @@
     <col min="11" max="11" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="E1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="E1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="J1" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="10"/>
-    </row>
-    <row r="2" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
@@ -653,24 +634,18 @@
         <v>2</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -679,192 +654,162 @@
         <v>-5182000</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="11">
+        <v>3</v>
+      </c>
+      <c r="H3" s="6">
         <v>44337</v>
       </c>
-      <c r="J3" s="5">
-        <v>1</v>
-      </c>
-      <c r="K3" s="5">
-        <v>1621555200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="3">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F4" s="3">
-        <v>-160000</v>
+        <v>500000</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="11">
-        <v>44427</v>
-      </c>
-      <c r="J4" s="5">
-        <v>2</v>
-      </c>
-      <c r="K4" s="5">
-        <v>1629331200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="H4" s="6">
+        <v>44340</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F5" s="3">
         <v>-50000</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="12">
-        <v>44484</v>
-      </c>
-      <c r="J5" s="5">
-        <v>3</v>
-      </c>
-      <c r="K5" s="5">
-        <v>1634256000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="H5" s="6">
+        <v>44345</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="3">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F6" s="3">
-        <v>500000</v>
+        <v>-160000</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="11">
-        <v>44340</v>
-      </c>
-      <c r="J6" s="7">
         <v>4</v>
       </c>
-      <c r="K6" s="3">
-        <v>1634342400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H6" s="6">
+        <v>44427</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="3">
-        <v>10</v>
-      </c>
-      <c r="F7" s="6">
-        <v>300000</v>
+        <v>2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>-50000</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="11">
-        <v>44485</v>
-      </c>
-      <c r="J7" s="7">
         <v>5</v>
       </c>
-      <c r="K7" s="3">
-        <v>1635120000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H7" s="7">
+        <v>44484</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" s="3">
-        <v>10000</v>
+        <v>1200000</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="11">
-        <v>44494</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="H8" s="6">
+        <v>44484</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="3">
-        <v>8</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1200000</v>
+        <v>10</v>
+      </c>
+      <c r="F9" s="5">
+        <v>300000</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="13">
-        <v>44484</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="H9" s="8">
+        <v>44485</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="3">
@@ -874,45 +819,45 @@
         <v>-22000</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="11">
+        <v>28</v>
+      </c>
+      <c r="H10" s="6">
         <v>44485</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="3">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F11" s="3">
-        <v>-50000</v>
+        <v>10000</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="11">
-        <v>44345</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="H11" s="6">
+        <v>44494</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="3">
@@ -922,17 +867,19 @@
         <v>200000</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="11">
+        <v>29</v>
+      </c>
+      <c r="H12" s="6">
         <v>44494</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E3:H12">
+    <sortCondition ref="H3:H12"/>
+  </sortState>
+  <mergeCells count="2">
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>